<commit_message>
feito ate a 1.2
</commit_message>
<xml_diff>
--- a/Exercicios_02.08/1.3-exercicios-pclincs/1.3-exercicio-pclinics-fisico.xlsx
+++ b/Exercicios_02.08/1.3-exercicios-pclincs/1.3-exercicio-pclinics-fisico.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\2°semestre- SENAI\sprint-1_2-semestre\Exercicios_02.08\1.3-exercicios-pclincs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fic\Desktop\sprint-1_2-semestre\Exercicios_02.08\1.3-exercicios-pclincs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABC59844-EF48-4D8F-8F39-3BBEAD7A2920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE21DAF-EAB0-46E6-86B0-B238393EB60F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{92CA52D3-D9AD-4D32-B518-32793EB2E825}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11388" xr2:uid="{92CA52D3-D9AD-4D32-B518-32793EB2E825}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>dono</t>
   </si>
@@ -121,13 +121,16 @@
   </si>
   <si>
     <t>dataAtendimento</t>
+  </si>
+  <si>
+    <t>rua2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +145,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="23">
     <fill>
@@ -289,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -335,6 +346,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,24 +672,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B880A24-AF96-43FC-86CF-BC4A1EDC2A09}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +706,7 @@
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -723,7 +735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -752,7 +764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -781,7 +793,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E5" s="11">
         <v>3</v>
       </c>
@@ -796,15 +808,16 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -827,7 +840,7 @@
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -856,7 +869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -885,7 +898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>3</v>
       </c>
@@ -898,17 +911,23 @@
       <c r="D11" s="8">
         <v>44512</v>
       </c>
+      <c r="G11" s="17">
+        <v>2</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>32</v>
+      </c>
       <c r="K11" s="25">
         <v>2</v>
       </c>
       <c r="L11" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M11" s="26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>4</v>
       </c>
@@ -934,13 +953,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G15" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="G16" s="20" t="s">
         <v>24</v>
       </c>
@@ -948,7 +967,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G17" s="21">
         <v>1</v>
       </c>
@@ -956,9 +975,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.3">
       <c r="G18" s="21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>15</v>
@@ -966,5 +985,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>